<commit_message>
Optimierung der Schuelerzuweisung. Aussteht nur noch der Export und das Handeln mit Fehlerhaften Daten beim einlesen (Fehlende Veranstalltungen, Unternehmen, Wahlen etc.)
</commit_message>
<xml_diff>
--- a/Data/IMPORT_BOT1_Veranstaltungsliste.xlsx
+++ b/Data/IMPORT_BOT1_Veranstaltungsliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\+++Schule\AE_LF12\Projekt Berufsorientierungstag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SE\Schulprojekt\DPA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138B5649-8413-4F6E-9D0E-902A61ECF0DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC32794-E31F-47EB-9EDD-F662989A3889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{3A9E2240-F68F-4045-AE50-B76F133D2F1C}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{3A9E2240-F68F-4045-AE50-B76F133D2F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>Unternehmen</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t xml:space="preserve">StädteRegion Aachen </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finanzamt </t>
   </si>
   <si>
     <t xml:space="preserve">duales Studium Dipl. Finanzwirt/-in </t>
@@ -259,9 +256,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -299,7 +296,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -405,7 +402,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -547,7 +544,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -557,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6BCE577-6462-43C7-A707-99D40A5D160F}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,13 +580,13 @@
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -609,7 +606,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -629,7 +626,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -649,7 +646,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -660,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1">
         <v>20</v>
@@ -669,7 +666,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -689,7 +686,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -709,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -720,7 +717,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="1">
         <v>20</v>
@@ -729,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -749,7 +746,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -769,7 +766,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -789,7 +786,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -809,7 +806,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -829,7 +826,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -849,7 +846,7 @@
         <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -860,7 +857,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1">
         <v>20</v>
@@ -869,7 +866,7 @@
         <v>5</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -889,7 +886,7 @@
         <v>5</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -909,7 +906,7 @@
         <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -920,7 +917,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1">
         <v>20</v>
@@ -929,7 +926,7 @@
         <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -940,7 +937,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="1">
         <v>20</v>
@@ -949,7 +946,7 @@
         <v>5</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -957,10 +954,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="1">
         <v>20</v>
@@ -969,10 +966,10 @@
         <v>5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -980,7 +977,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="1">
         <v>20</v>
@@ -989,10 +986,10 @@
         <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1000,7 +997,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="1">
         <v>20</v>
@@ -1009,7 +1006,7 @@
         <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1020,7 +1017,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="1">
         <v>25</v>
@@ -1029,7 +1026,7 @@
         <v>5</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1046,7 +1043,7 @@
         <v>5</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1066,7 +1063,7 @@
         <v>5</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1083,7 +1080,7 @@
         <v>5</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,7 +1097,7 @@
         <v>5</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1117,7 +1114,7 @@
         <v>5</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raumzuweisung funktioniert. Es werden keine leeren Slots freigehalten.
</commit_message>
<xml_diff>
--- a/Data/IMPORT_BOT1_Veranstaltungsliste.xlsx
+++ b/Data/IMPORT_BOT1_Veranstaltungsliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex-\Desktop\Schulprojekt\DPA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434E1DE6-C5C8-4751-A5FC-38F5992CF9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBDC459-9C51-49CD-A0E2-36675188D15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15345" xr2:uid="{3A9E2240-F68F-4045-AE50-B76F133D2F1C}"/>
   </bookViews>
@@ -554,7 +554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6BCE577-6462-43C7-A707-99D40A5D160F}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>